<commit_message>
updated datastructure testdata xlsx
</commit_message>
<xml_diff>
--- a/testdata/ds-algo-testdata.xlsx
+++ b/testdata/ds-algo-testdata.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>password1</t>
   </si>
@@ -29,6 +29,12 @@
   </si>
   <si>
     <t>viji #12</t>
+  </si>
+  <si>
+    <t>viji@123</t>
+  </si>
+  <si>
+    <t>vijayarani</t>
   </si>
 </sst>
 </file>
@@ -321,8 +327,15 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>